<commit_message>
Changed flow and completed up to section 4 excluding references
</commit_message>
<xml_diff>
--- a/paper/Workbook1.xlsx
+++ b/paper/Workbook1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24000" yWindow="80" windowWidth="24000" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,8 +200,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,7 +284,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -321,6 +323,7 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -359,6 +362,7 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="R23" sqref="M18:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -997,15 +1001,73 @@
         <v>25.57</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="18" spans="1:18">
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="M19">
+        <v>0.84147099999999997</v>
+      </c>
+      <c r="N19">
+        <v>0.84147099999999997</v>
+      </c>
+      <c r="O19">
+        <v>0.84147099999999997</v>
+      </c>
+      <c r="P19">
+        <v>0.84147099999999997</v>
+      </c>
+      <c r="Q19">
+        <v>0.84147099999999997</v>
+      </c>
+      <c r="R19">
+        <v>0.84147099999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="M20">
+        <v>0.90929700000000002</v>
+      </c>
+      <c r="N20">
+        <v>0.90929700000000002</v>
+      </c>
+      <c r="O20">
+        <v>0.90929700000000002</v>
+      </c>
+      <c r="P20">
+        <v>0.90929700000000002</v>
+      </c>
+      <c r="Q20">
+        <v>0.90929700000000002</v>
+      </c>
+      <c r="R20">
+        <v>0.90929700000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1018,8 +1080,26 @@
       <c r="D21">
         <v>117.87</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="M21">
+        <v>0.14112</v>
+      </c>
+      <c r="N21">
+        <v>0.14112</v>
+      </c>
+      <c r="O21">
+        <v>0.14112</v>
+      </c>
+      <c r="P21">
+        <v>0.14112</v>
+      </c>
+      <c r="Q21">
+        <v>0.14112</v>
+      </c>
+      <c r="R21">
+        <v>0.14112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1047,8 +1127,26 @@
       <c r="I22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="M22">
+        <v>-0.75680199999999997</v>
+      </c>
+      <c r="N22">
+        <v>-0.75680199999999997</v>
+      </c>
+      <c r="O22">
+        <v>-0.75680199999999997</v>
+      </c>
+      <c r="P22">
+        <v>-0.75680199999999997</v>
+      </c>
+      <c r="Q22">
+        <v>-0.75680199999999997</v>
+      </c>
+      <c r="R22">
+        <v>-0.75680199999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1076,8 +1174,26 @@
       <c r="I23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="M23">
+        <v>-0.958924</v>
+      </c>
+      <c r="N23">
+        <v>-0.958924</v>
+      </c>
+      <c r="O23">
+        <v>-0.958924</v>
+      </c>
+      <c r="P23">
+        <v>-0.958924</v>
+      </c>
+      <c r="Q23">
+        <v>-0.958924</v>
+      </c>
+      <c r="R23">
+        <v>-0.958924</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1106,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1128,7 +1244,7 @@
         <v>86.9</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1142,11 +1258,11 @@
         <v>93.46</v>
       </c>
       <c r="F28">
-        <f>$B$27/B28</f>
+        <f t="shared" ref="F28:F34" si="9">$B$27/B28</f>
         <v>1.4668133480014669</v>
       </c>
       <c r="G28">
-        <f>$C$27/C28</f>
+        <f t="shared" ref="G28:G34" si="10">$C$27/C28</f>
         <v>1.3825363825363828</v>
       </c>
       <c r="H28">
@@ -1157,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1171,22 +1287,22 @@
         <v>97.68</v>
       </c>
       <c r="F29">
-        <f>$B$27/B29</f>
+        <f t="shared" si="9"/>
         <v>1.7559262510974538</v>
       </c>
       <c r="G29">
-        <f>$C$27/C29</f>
+        <f t="shared" si="10"/>
         <v>1.6419753086419755</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:H34" si="9">$D$27/D29</f>
+        <f t="shared" ref="H29:H34" si="11">$D$27/D29</f>
         <v>0.88963963963963966</v>
       </c>
       <c r="I29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1200,22 +1316,22 @@
         <v>104.65</v>
       </c>
       <c r="F30">
-        <f>$B$27/B30</f>
+        <f t="shared" si="9"/>
         <v>2.5673940949935816</v>
       </c>
       <c r="G30">
-        <f>$C$27/C30</f>
+        <f t="shared" si="10"/>
         <v>2.3835125448028673</v>
       </c>
       <c r="H30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.83038700430004775</v>
       </c>
       <c r="I30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:18">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1229,22 +1345,22 @@
         <v>107.3</v>
       </c>
       <c r="F31">
-        <f>$B$27/B31</f>
+        <f t="shared" si="9"/>
         <v>2.8089887640449436</v>
       </c>
       <c r="G31">
-        <f>$C$27/C31</f>
+        <f t="shared" si="10"/>
         <v>2.5775193798449614</v>
       </c>
       <c r="H31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.80987884436160307</v>
       </c>
       <c r="I31">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1258,15 +1374,15 @@
         <v>114.56</v>
       </c>
       <c r="F32">
-        <f>$B$27/B32</f>
+        <f t="shared" si="9"/>
         <v>3.3528918692372174</v>
       </c>
       <c r="G32">
-        <f>$C$27/C32</f>
+        <f t="shared" si="10"/>
         <v>2.9424778761061949</v>
       </c>
       <c r="H32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.75855446927374304</v>
       </c>
       <c r="I32">
@@ -1287,15 +1403,15 @@
         <v>113.44</v>
       </c>
       <c r="F33">
-        <f>$B$27/B33</f>
+        <f t="shared" si="9"/>
         <v>3.6596523330283626</v>
       </c>
       <c r="G33">
-        <f>$C$27/C33</f>
+        <f t="shared" si="10"/>
         <v>3.3250000000000002</v>
       </c>
       <c r="H33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.76604372355430195</v>
       </c>
       <c r="I33">
@@ -1316,15 +1432,15 @@
         <v>124.02</v>
       </c>
       <c r="F34">
-        <f>$B$27/B34</f>
+        <f t="shared" si="9"/>
         <v>4.509582863585119</v>
       </c>
       <c r="G34">
-        <f>$C$27/C34</f>
+        <f t="shared" si="10"/>
         <v>3.5000000000000004</v>
       </c>
       <c r="H34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.70069343654249316</v>
       </c>
       <c r="I34">
@@ -1559,15 +1675,15 @@
         <v>0.28000000000001535</v>
       </c>
       <c r="C59">
-        <f t="shared" ref="C59:E59" si="10">C58-C57-C56</f>
+        <f t="shared" ref="C59:E59" si="12">C58-C57-C56</f>
         <v>0.40000000000000568</v>
       </c>
       <c r="D59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9.9999999999980105E-3</v>
       </c>
       <c r="E59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-7.9999999999998295E-2</v>
       </c>
     </row>

</xml_diff>